<commit_message>
commit on augugst 20 2020
</commit_message>
<xml_diff>
--- a/Input_data/Copied_data/new_copied_data3106.xlsx
+++ b/Input_data/Copied_data/new_copied_data3106.xlsx
@@ -9,21 +9,25 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" tabRatio="772" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sort By &amp; Total by Check #" sheetId="6" r:id="rId1"/>
-    <sheet name="Formating-Prelim" sheetId="5" r:id="rId2"/>
-    <sheet name="Identify Replacements" sheetId="4" r:id="rId3"/>
-    <sheet name="Elim Col A to D &amp; Sort by Chk #" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId5"/>
+    <sheet name="Report_final1" sheetId="14" r:id="rId1"/>
+    <sheet name="Sort By &amp; Total by Check #" sheetId="6" r:id="rId2"/>
+    <sheet name="Formating-Prelim" sheetId="5" r:id="rId3"/>
+    <sheet name="Identify Replacements" sheetId="4" r:id="rId4"/>
+    <sheet name="Elim Col A to D &amp; Sort by Chk #" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sort By &amp; Total by Check #'!$A$1:$L$19</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2123" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2134" uniqueCount="374">
   <si>
     <t>Column1</t>
   </si>
@@ -1105,7 +1109,46 @@
     <t>K-3085169</t>
   </si>
   <si>
-    <t xml:space="preserve"> Chk Amt</t>
+    <t>Sum_Amount</t>
+  </si>
+  <si>
+    <t>carpet replace</t>
+  </si>
+  <si>
+    <t>dishwasher</t>
+  </si>
+  <si>
+    <t>water heater replace</t>
+  </si>
+  <si>
+    <t>ac replace</t>
+  </si>
+  <si>
+    <t>fridge replace</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>Payee_Name</t>
+  </si>
+  <si>
+    <t>Check_Date</t>
+  </si>
+  <si>
+    <t>Invoice_Date</t>
+  </si>
+  <si>
+    <t>System_Method</t>
+  </si>
+  <si>
+    <t>check_control</t>
+  </si>
+  <si>
+    <t>Chk_Amt</t>
   </si>
 </sst>
 </file>
@@ -1447,690 +1490,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A6:L24"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B2">
+        <v>4347</v>
+      </c>
+      <c r="C2">
+        <v>190.96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B3">
+        <v>4389</v>
+      </c>
+      <c r="C3">
+        <v>269.26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>363</v>
+      </c>
+      <c r="B4">
+        <v>4389</v>
+      </c>
+      <c r="C4">
+        <v>2091.46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>365</v>
+      </c>
+      <c r="B5">
+        <v>4389</v>
+      </c>
+      <c r="C5">
+        <v>531.04999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>345</v>
-      </c>
-      <c r="B6" t="s">
-        <v>346</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>347</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" t="s">
-        <v>348</v>
-      </c>
-      <c r="I6" t="s">
-        <v>349</v>
-      </c>
-      <c r="J6" t="s">
-        <v>360</v>
-      </c>
-      <c r="K6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+      <c r="B6">
+        <v>4389</v>
+      </c>
+      <c r="C6">
+        <v>913.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>363</v>
       </c>
       <c r="B7">
-        <v>13780</v>
+        <v>4448</v>
       </c>
       <c r="C7">
-        <v>1851526</v>
-      </c>
-      <c r="D7" s="3">
-        <v>43263</v>
-      </c>
-      <c r="E7" s="3">
-        <v>43344</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7">
-        <v>190.96</v>
-      </c>
-      <c r="H7" t="s">
-        <v>151</v>
-      </c>
-      <c r="I7">
-        <v>4347</v>
-      </c>
-      <c r="J7">
-        <v>190.96</v>
-      </c>
-      <c r="K7" s="3">
-        <v>43271</v>
-      </c>
-      <c r="L7" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1416.69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>364</v>
       </c>
       <c r="B8">
-        <v>13780</v>
+        <v>4448</v>
       </c>
       <c r="C8">
-        <v>9164332949</v>
-      </c>
-      <c r="D8" s="3">
-        <v>43283</v>
-      </c>
-      <c r="E8" s="3">
-        <v>43282</v>
-      </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8">
-        <v>269.26</v>
-      </c>
-      <c r="H8" t="s">
-        <v>223</v>
-      </c>
-      <c r="I8">
-        <v>4389</v>
-      </c>
-      <c r="K8" s="3">
-        <v>43293</v>
-      </c>
-      <c r="L8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1826.06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>363</v>
       </c>
       <c r="B9">
-        <v>13780</v>
+        <v>4470</v>
       </c>
       <c r="C9">
-        <v>9164332950</v>
-      </c>
-      <c r="D9" s="3">
-        <v>43283</v>
-      </c>
-      <c r="E9" s="3">
-        <v>43282</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9">
-        <v>403.51</v>
-      </c>
-      <c r="H9" t="s">
-        <v>223</v>
-      </c>
-      <c r="I9">
-        <v>4389</v>
-      </c>
-      <c r="K9" s="3">
-        <v>43293</v>
-      </c>
-      <c r="L9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>13780</v>
-      </c>
-      <c r="C10">
-        <v>9164332948</v>
-      </c>
-      <c r="D10" s="3">
-        <v>43283</v>
-      </c>
-      <c r="E10" s="3">
-        <v>43282</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10">
-        <v>403.51</v>
-      </c>
-      <c r="H10" t="s">
-        <v>223</v>
-      </c>
-      <c r="I10">
-        <v>4389</v>
-      </c>
-      <c r="K10" s="3">
-        <v>43293</v>
-      </c>
-      <c r="L10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>13780</v>
-      </c>
-      <c r="C11">
-        <v>9164332951</v>
-      </c>
-      <c r="D11" s="3">
-        <v>43283</v>
-      </c>
-      <c r="E11" s="3">
-        <v>43282</v>
-      </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11">
-        <v>403.51</v>
-      </c>
-      <c r="H11" t="s">
-        <v>223</v>
-      </c>
-      <c r="I11">
-        <v>4389</v>
-      </c>
-      <c r="K11" s="3">
-        <v>43293</v>
-      </c>
-      <c r="L11" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>13780</v>
-      </c>
-      <c r="C12">
-        <v>9164332948</v>
-      </c>
-      <c r="D12" s="3">
-        <v>43283</v>
-      </c>
-      <c r="E12" s="3">
-        <v>43282</v>
-      </c>
-      <c r="F12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12">
-        <v>440.46</v>
-      </c>
-      <c r="H12" t="s">
-        <v>352</v>
-      </c>
-      <c r="I12">
-        <v>4389</v>
-      </c>
-      <c r="K12" s="3">
-        <v>43293</v>
-      </c>
-      <c r="L12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13">
-        <v>13780</v>
-      </c>
-      <c r="C13">
-        <v>9164332950</v>
-      </c>
-      <c r="D13" s="3">
-        <v>43283</v>
-      </c>
-      <c r="E13" s="3">
-        <v>43282</v>
-      </c>
-      <c r="F13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13">
-        <v>440.47</v>
-      </c>
-      <c r="H13" t="s">
-        <v>223</v>
-      </c>
-      <c r="I13">
-        <v>4389</v>
-      </c>
-      <c r="K13" s="3">
-        <v>43293</v>
-      </c>
-      <c r="L13" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>13780</v>
-      </c>
-      <c r="C14">
-        <v>9164332951</v>
-      </c>
-      <c r="D14" s="3">
-        <v>43283</v>
-      </c>
-      <c r="E14" s="3">
-        <v>43282</v>
-      </c>
-      <c r="F14" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14">
-        <v>531.04999999999995</v>
-      </c>
-      <c r="H14" t="s">
-        <v>223</v>
-      </c>
-      <c r="I14">
-        <v>4389</v>
-      </c>
-      <c r="K14" s="3">
-        <v>43293</v>
-      </c>
-      <c r="L14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>13780</v>
-      </c>
-      <c r="C15">
-        <v>9164332950</v>
-      </c>
-      <c r="D15" s="3">
-        <v>43283</v>
-      </c>
-      <c r="E15" s="3">
-        <v>43282</v>
-      </c>
-      <c r="F15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15">
-        <v>913.01</v>
-      </c>
-      <c r="H15" t="s">
-        <v>223</v>
-      </c>
-      <c r="I15">
-        <v>4389</v>
-      </c>
-      <c r="J15">
-        <v>3804.78</v>
-      </c>
-      <c r="K15" s="3">
-        <v>43293</v>
-      </c>
-      <c r="L15" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>13780</v>
-      </c>
-      <c r="C16">
-        <v>9164783846</v>
-      </c>
-      <c r="D16" s="3">
-        <v>43300</v>
-      </c>
-      <c r="E16" s="3">
-        <v>43313</v>
-      </c>
-      <c r="F16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16">
-        <v>446.3</v>
-      </c>
-      <c r="H16" t="s">
-        <v>39</v>
-      </c>
-      <c r="I16">
-        <v>4448</v>
-      </c>
-      <c r="K16" s="3">
-        <v>43321</v>
-      </c>
-      <c r="L16" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>13780</v>
-      </c>
-      <c r="C17">
-        <v>9164783845</v>
-      </c>
-      <c r="D17" s="3">
-        <v>43300</v>
-      </c>
-      <c r="E17" s="3">
-        <v>43313</v>
-      </c>
-      <c r="F17" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17">
-        <v>485.19</v>
-      </c>
-      <c r="H17" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17">
-        <v>4448</v>
-      </c>
-      <c r="K17" s="3">
-        <v>43321</v>
-      </c>
-      <c r="L17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18">
-        <v>13780</v>
-      </c>
-      <c r="C18">
-        <v>9164896693</v>
-      </c>
-      <c r="D18" s="3">
-        <v>43305</v>
-      </c>
-      <c r="E18" s="3">
-        <v>43313</v>
-      </c>
-      <c r="F18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18">
-        <v>485.2</v>
-      </c>
-      <c r="H18" t="s">
-        <v>39</v>
-      </c>
-      <c r="I18">
-        <v>4448</v>
-      </c>
-      <c r="K18" s="3">
-        <v>43321</v>
-      </c>
-      <c r="L18" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19">
-        <v>13780</v>
-      </c>
-      <c r="C19">
-        <v>9164823334</v>
-      </c>
-      <c r="D19" s="3">
-        <v>43301</v>
-      </c>
-      <c r="E19" s="3">
-        <v>43313</v>
-      </c>
-      <c r="F19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19">
-        <v>913.02</v>
-      </c>
-      <c r="H19" t="s">
-        <v>39</v>
-      </c>
-      <c r="I19">
-        <v>4448</v>
-      </c>
-      <c r="K19" s="3">
-        <v>43321</v>
-      </c>
-      <c r="L19" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20">
-        <v>13780</v>
-      </c>
-      <c r="C20">
-        <v>9164933879</v>
-      </c>
-      <c r="D20" s="3">
-        <v>43306</v>
-      </c>
-      <c r="E20" s="3">
-        <v>43313</v>
-      </c>
-      <c r="F20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20">
-        <v>913.04</v>
-      </c>
-      <c r="H20" t="s">
-        <v>39</v>
-      </c>
-      <c r="I20">
-        <v>4448</v>
-      </c>
-      <c r="J20">
-        <v>3242.75</v>
-      </c>
-      <c r="K20" s="3">
-        <v>43321</v>
-      </c>
-      <c r="L20" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21">
-        <v>13780</v>
-      </c>
-      <c r="C21">
-        <v>9165138617</v>
-      </c>
-      <c r="D21" s="3">
-        <v>43313</v>
-      </c>
-      <c r="E21" s="3">
-        <v>43313</v>
-      </c>
-      <c r="F21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21">
-        <v>446.3</v>
-      </c>
-      <c r="H21" t="s">
-        <v>356</v>
-      </c>
-      <c r="I21">
-        <v>4470</v>
-      </c>
-      <c r="K21" s="3">
-        <v>43328</v>
-      </c>
-      <c r="L21" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22">
-        <v>13780</v>
-      </c>
-      <c r="C22">
-        <v>9165169652</v>
-      </c>
-      <c r="D22" s="3">
-        <v>43314</v>
-      </c>
-      <c r="E22" s="3">
-        <v>43313</v>
-      </c>
-      <c r="F22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22">
-        <v>446.32</v>
-      </c>
-      <c r="H22" t="s">
-        <v>49</v>
-      </c>
-      <c r="I22">
-        <v>4470</v>
-      </c>
-      <c r="K22" s="3">
-        <v>43328</v>
-      </c>
-      <c r="L22" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23">
-        <v>13780</v>
-      </c>
-      <c r="C23">
-        <v>9165295619</v>
-      </c>
-      <c r="D23" s="3">
-        <v>43319</v>
-      </c>
-      <c r="E23" s="3">
-        <v>43313</v>
-      </c>
-      <c r="F23" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23">
-        <v>485.2</v>
-      </c>
-      <c r="H23" t="s">
-        <v>359</v>
-      </c>
-      <c r="I23">
-        <v>4470</v>
-      </c>
-      <c r="K23" s="3">
-        <v>43328</v>
-      </c>
-      <c r="L23" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24">
-        <v>13780</v>
-      </c>
-      <c r="C24">
-        <v>9165169658</v>
-      </c>
-      <c r="D24" s="3">
-        <v>43314</v>
-      </c>
-      <c r="E24" s="3">
-        <v>43313</v>
-      </c>
-      <c r="F24" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24">
-        <v>892.6</v>
-      </c>
-      <c r="H24" t="s">
-        <v>49</v>
-      </c>
-      <c r="I24">
-        <v>4470</v>
-      </c>
-      <c r="J24">
         <v>2270.42</v>
-      </c>
-      <c r="K24" s="3">
-        <v>43328</v>
-      </c>
-      <c r="L24" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2139,6 +1605,757 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D1" t="s">
+        <v>370</v>
+      </c>
+      <c r="E1" t="s">
+        <v>347</v>
+      </c>
+      <c r="F1" t="s">
+        <v>371</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I1" t="s">
+        <v>349</v>
+      </c>
+      <c r="J1" t="s">
+        <v>373</v>
+      </c>
+      <c r="K1" t="s">
+        <v>369</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2">
+        <v>13780</v>
+      </c>
+      <c r="C2">
+        <v>1851526</v>
+      </c>
+      <c r="D2" s="3">
+        <v>43263</v>
+      </c>
+      <c r="E2" s="3">
+        <v>43344</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2">
+        <v>190.96</v>
+      </c>
+      <c r="H2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I2">
+        <v>4347</v>
+      </c>
+      <c r="J2">
+        <v>190.96</v>
+      </c>
+      <c r="K2" s="3">
+        <v>43271</v>
+      </c>
+      <c r="L2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>13780</v>
+      </c>
+      <c r="C3">
+        <v>9164332949</v>
+      </c>
+      <c r="D3" s="3">
+        <v>43283</v>
+      </c>
+      <c r="E3" s="3">
+        <v>43282</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3">
+        <v>269.26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>223</v>
+      </c>
+      <c r="I3">
+        <v>4389</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>43293</v>
+      </c>
+      <c r="L3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>13780</v>
+      </c>
+      <c r="C4">
+        <v>9164332950</v>
+      </c>
+      <c r="D4" s="3">
+        <v>43283</v>
+      </c>
+      <c r="E4" s="3">
+        <v>43282</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4">
+        <v>403.51</v>
+      </c>
+      <c r="H4" t="s">
+        <v>223</v>
+      </c>
+      <c r="I4">
+        <v>4389</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3">
+        <v>43293</v>
+      </c>
+      <c r="L4" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>13780</v>
+      </c>
+      <c r="C5">
+        <v>9164332948</v>
+      </c>
+      <c r="D5" s="3">
+        <v>43283</v>
+      </c>
+      <c r="E5" s="3">
+        <v>43282</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5">
+        <v>403.51</v>
+      </c>
+      <c r="H5" t="s">
+        <v>223</v>
+      </c>
+      <c r="I5">
+        <v>4389</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>43293</v>
+      </c>
+      <c r="L5" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>13780</v>
+      </c>
+      <c r="C6">
+        <v>9164332951</v>
+      </c>
+      <c r="D6" s="3">
+        <v>43283</v>
+      </c>
+      <c r="E6" s="3">
+        <v>43282</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6">
+        <v>403.51</v>
+      </c>
+      <c r="H6" t="s">
+        <v>223</v>
+      </c>
+      <c r="I6">
+        <v>4389</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>43293</v>
+      </c>
+      <c r="L6" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>13780</v>
+      </c>
+      <c r="C7">
+        <v>9164332948</v>
+      </c>
+      <c r="D7" s="3">
+        <v>43283</v>
+      </c>
+      <c r="E7" s="3">
+        <v>43282</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7">
+        <v>440.46</v>
+      </c>
+      <c r="H7" t="s">
+        <v>352</v>
+      </c>
+      <c r="I7">
+        <v>4389</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>43293</v>
+      </c>
+      <c r="L7" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>13780</v>
+      </c>
+      <c r="C8">
+        <v>9164332950</v>
+      </c>
+      <c r="D8" s="3">
+        <v>43283</v>
+      </c>
+      <c r="E8" s="3">
+        <v>43282</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8">
+        <v>440.47</v>
+      </c>
+      <c r="H8" t="s">
+        <v>223</v>
+      </c>
+      <c r="I8">
+        <v>4389</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>43293</v>
+      </c>
+      <c r="L8" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>13780</v>
+      </c>
+      <c r="C9">
+        <v>9164332951</v>
+      </c>
+      <c r="D9" s="3">
+        <v>43283</v>
+      </c>
+      <c r="E9" s="3">
+        <v>43282</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9">
+        <v>531.04999999999995</v>
+      </c>
+      <c r="H9" t="s">
+        <v>223</v>
+      </c>
+      <c r="I9">
+        <v>4389</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <v>43293</v>
+      </c>
+      <c r="L9" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>13780</v>
+      </c>
+      <c r="C10">
+        <v>9164332950</v>
+      </c>
+      <c r="D10" s="3">
+        <v>43283</v>
+      </c>
+      <c r="E10" s="3">
+        <v>43282</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10">
+        <v>913.01</v>
+      </c>
+      <c r="H10" t="s">
+        <v>223</v>
+      </c>
+      <c r="I10">
+        <v>4389</v>
+      </c>
+      <c r="J10">
+        <v>3804.78</v>
+      </c>
+      <c r="K10" s="3">
+        <v>43293</v>
+      </c>
+      <c r="L10" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>13780</v>
+      </c>
+      <c r="C11">
+        <v>9164783846</v>
+      </c>
+      <c r="D11" s="3">
+        <v>43300</v>
+      </c>
+      <c r="E11" s="3">
+        <v>43313</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11">
+        <v>446.3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11">
+        <v>4448</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>43321</v>
+      </c>
+      <c r="L11" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>13780</v>
+      </c>
+      <c r="C12">
+        <v>9164783845</v>
+      </c>
+      <c r="D12" s="3">
+        <v>43300</v>
+      </c>
+      <c r="E12" s="3">
+        <v>43313</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12">
+        <v>485.19</v>
+      </c>
+      <c r="H12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12">
+        <v>4448</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3">
+        <v>43321</v>
+      </c>
+      <c r="L12" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>13780</v>
+      </c>
+      <c r="C13">
+        <v>9164896693</v>
+      </c>
+      <c r="D13" s="3">
+        <v>43305</v>
+      </c>
+      <c r="E13" s="3">
+        <v>43313</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13">
+        <v>485.2</v>
+      </c>
+      <c r="H13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13">
+        <v>4448</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="3">
+        <v>43321</v>
+      </c>
+      <c r="L13" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>13780</v>
+      </c>
+      <c r="C14">
+        <v>9164823334</v>
+      </c>
+      <c r="D14" s="3">
+        <v>43301</v>
+      </c>
+      <c r="E14" s="3">
+        <v>43313</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14">
+        <v>913.02</v>
+      </c>
+      <c r="H14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14">
+        <v>4448</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>43321</v>
+      </c>
+      <c r="L14" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>13780</v>
+      </c>
+      <c r="C15">
+        <v>9164933879</v>
+      </c>
+      <c r="D15" s="3">
+        <v>43306</v>
+      </c>
+      <c r="E15" s="3">
+        <v>43313</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15">
+        <v>913.04</v>
+      </c>
+      <c r="H15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15">
+        <v>4448</v>
+      </c>
+      <c r="J15">
+        <v>3242.75</v>
+      </c>
+      <c r="K15" s="3">
+        <v>43321</v>
+      </c>
+      <c r="L15" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>13780</v>
+      </c>
+      <c r="C16">
+        <v>9165138617</v>
+      </c>
+      <c r="D16" s="3">
+        <v>43313</v>
+      </c>
+      <c r="E16" s="3">
+        <v>43313</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16">
+        <v>446.3</v>
+      </c>
+      <c r="H16" t="s">
+        <v>356</v>
+      </c>
+      <c r="I16">
+        <v>4470</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16" s="3">
+        <v>43328</v>
+      </c>
+      <c r="L16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>13780</v>
+      </c>
+      <c r="C17">
+        <v>9165169652</v>
+      </c>
+      <c r="D17" s="3">
+        <v>43314</v>
+      </c>
+      <c r="E17" s="3">
+        <v>43313</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17">
+        <v>446.32</v>
+      </c>
+      <c r="H17" t="s">
+        <v>49</v>
+      </c>
+      <c r="I17">
+        <v>4470</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17" s="3">
+        <v>43328</v>
+      </c>
+      <c r="L17" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>13780</v>
+      </c>
+      <c r="C18">
+        <v>9165295619</v>
+      </c>
+      <c r="D18" s="3">
+        <v>43319</v>
+      </c>
+      <c r="E18" s="3">
+        <v>43313</v>
+      </c>
+      <c r="F18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18">
+        <v>485.2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>359</v>
+      </c>
+      <c r="I18">
+        <v>4470</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18" s="3">
+        <v>43328</v>
+      </c>
+      <c r="L18" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>13780</v>
+      </c>
+      <c r="C19">
+        <v>9165169658</v>
+      </c>
+      <c r="D19" s="3">
+        <v>43314</v>
+      </c>
+      <c r="E19" s="3">
+        <v>43313</v>
+      </c>
+      <c r="F19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19">
+        <v>892.6</v>
+      </c>
+      <c r="H19" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19">
+        <v>4470</v>
+      </c>
+      <c r="J19">
+        <v>2270.42</v>
+      </c>
+      <c r="K19" s="3">
+        <v>43328</v>
+      </c>
+      <c r="L19" t="s">
+        <v>363</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:K24"/>
   <sheetViews>
@@ -2816,7 +3033,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K42"/>
   <sheetViews>
@@ -4299,7 +4516,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O135"/>
   <sheetViews>
@@ -10019,7 +10236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O164"/>
   <sheetViews>

</xml_diff>